<commit_message>
Update: Fix CI/CD script, cleanup files, and retrain models
</commit_message>
<xml_diff>
--- a/data/raw/DATA RUMAH.xlsx
+++ b/data/raw/DATA RUMAH.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1052"/>
+  <dimension ref="A1:H1085"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28677,23 +28677,23 @@
       </c>
       <c r="B1009" t="inlineStr">
         <is>
-          <t>Nivara Resort Townhouse at Wijaya</t>
+          <t>Dijual Cepat Alam Segar Pondok Indah Harga Murah Semi Furnished Bagus, Rumah Pondok Indah</t>
         </is>
       </c>
       <c r="C1009" t="n">
-        <v>7090000000</v>
+        <v>11500000000</v>
       </c>
       <c r="D1009" t="n">
-        <v>375</v>
+        <v>310</v>
       </c>
       <c r="E1009" t="n">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="F1009" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1009" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1009" t="n">
         <v>1</v>
@@ -28705,26 +28705,26 @@
       </c>
       <c r="B1010" t="inlineStr">
         <is>
-          <t>Dijual Cepat Alam Segar Pondok Indah Harga Murah Semi Furnished Bagus, Rumah Pondok Indah</t>
+          <t>Rumah Classic Modern Siap Huni Fully Furnish Jual Cepat Jarang Ada Area Bebas Banjir</t>
         </is>
       </c>
       <c r="C1010" t="n">
-        <v>11500000000</v>
+        <v>38000000000</v>
       </c>
       <c r="D1010" t="n">
-        <v>310</v>
+        <v>760</v>
       </c>
       <c r="E1010" t="n">
-        <v>260</v>
+        <v>517</v>
       </c>
       <c r="F1010" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1010" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1010" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1011">
@@ -28733,26 +28733,26 @@
       </c>
       <c r="B1011" t="inlineStr">
         <is>
-          <t>Rumah Classic Modern Siap Huni Fully Furnish Jual Cepat Jarang Ada Area Bebas Banjir</t>
+          <t>Rumah Konsep Modern Elegan &amp; Sangat Hommy Siap Huni Bebas Banjir Kawasan Super Elite Kebayoran Baru Area Dharmawangsa</t>
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>38000000000</v>
+        <v>85000000000</v>
       </c>
       <c r="D1011" t="n">
-        <v>760</v>
+        <v>1500</v>
       </c>
       <c r="E1011" t="n">
-        <v>517</v>
+        <v>634</v>
       </c>
       <c r="F1011" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G1011" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1011" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1012">
@@ -28761,26 +28761,26 @@
       </c>
       <c r="B1012" t="inlineStr">
         <is>
-          <t>Rumah Konsep Modern Elegan &amp; Sangat Hommy Siap Huni Bebas Banjir Kawasan Super Elite Kebayoran Baru Area Dharmawangsa</t>
+          <t>Rumah Cozy Dn Nyaman di Lingkungan Pusat Bisnis di Fatmawati,Jakarta Selatan</t>
         </is>
       </c>
       <c r="C1012" t="n">
-        <v>85000000000</v>
+        <v>5200000000</v>
       </c>
       <c r="D1012" t="n">
-        <v>1500</v>
+        <v>215</v>
       </c>
       <c r="E1012" t="n">
-        <v>634</v>
+        <v>215</v>
       </c>
       <c r="F1012" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1012" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H1012" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1013">
@@ -28789,26 +28789,26 @@
       </c>
       <c r="B1013" t="inlineStr">
         <is>
-          <t>Rumah Cozy Dn Nyaman di Lingkungan Pusat Bisnis di Fatmawati,Jakarta Selatan</t>
+          <t>Rumah Lokasi Langka Wijaya 2 Super Strategis Lihat Jamin Beli</t>
         </is>
       </c>
       <c r="C1013" t="n">
-        <v>5200000000</v>
+        <v>20000000000</v>
       </c>
       <c r="D1013" t="n">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="E1013" t="n">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="F1013" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G1013" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H1013" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1014">
@@ -28817,26 +28817,26 @@
       </c>
       <c r="B1014" t="inlineStr">
         <is>
-          <t>Rumah Lokasi Langka Wijaya 2 Super Strategis Lihat Jamin Beli</t>
+          <t>For Sale Rumah Mewah Kondisi Baru Paling Strategis di Jakarta Selatan</t>
         </is>
       </c>
       <c r="C1014" t="n">
-        <v>20000000000</v>
+        <v>6900000000</v>
       </c>
       <c r="D1014" t="n">
-        <v>90</v>
+        <v>375</v>
       </c>
       <c r="E1014" t="n">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="F1014" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1014" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1014" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1015">
@@ -28845,17 +28845,17 @@
       </c>
       <c r="B1015" t="inlineStr">
         <is>
-          <t>For Sale Rumah Mewah Kondisi Baru Paling Strategis di Jakarta Selatan</t>
+          <t>Dijual Rumah Mewah 5 Lantai Ada Lift Interior Premium Designtropical Modern Di Pondok Indah Niaga Design By Ateiler Riri</t>
         </is>
       </c>
       <c r="C1015" t="n">
-        <v>6900000000</v>
+        <v>17500000000</v>
       </c>
       <c r="D1015" t="n">
-        <v>375</v>
+        <v>603</v>
       </c>
       <c r="E1015" t="n">
-        <v>76</v>
+        <v>264</v>
       </c>
       <c r="F1015" t="n">
         <v>4</v>
@@ -28873,26 +28873,26 @@
       </c>
       <c r="B1016" t="inlineStr">
         <is>
-          <t>ZENITPARC HYATT</t>
+          <t>For Sale Rumah Mewah 4 Lantai Kondisi Baru di Pusat Jakarta Selatan Dekat SCBD Senopati</t>
         </is>
       </c>
       <c r="C1016" t="n">
-        <v>2400000000</v>
+        <v>6900000000</v>
       </c>
       <c r="D1016" t="n">
-        <v>130</v>
+        <v>375</v>
       </c>
       <c r="E1016" t="n">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="F1016" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1016" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1016" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1017">
@@ -28901,26 +28901,26 @@
       </c>
       <c r="B1017" t="inlineStr">
         <is>
-          <t>Dijual Rumah Mewah 5 Lantai Ada Lift Interior Premium Designtropical Modern Di Pondok Indah Niaga Design By Ateiler Riri</t>
+          <t>Rumah Senopati Kebayoran Baru Rumah di Senopati SHM</t>
         </is>
       </c>
       <c r="C1017" t="n">
-        <v>17500000000</v>
+        <v>15500000000</v>
       </c>
       <c r="D1017" t="n">
-        <v>603</v>
+        <v>147</v>
       </c>
       <c r="E1017" t="n">
-        <v>264</v>
+        <v>317</v>
       </c>
       <c r="F1017" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1017" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1017" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1018">
@@ -28929,26 +28929,26 @@
       </c>
       <c r="B1018" t="inlineStr">
         <is>
-          <t>Dijual Rumah Di Tebet Barat Dalam Akses 2 Mobil Tebet Barat Jaksel</t>
+          <t>For Sale Rumah Mewah 4 Lantai Kondisi Baru di Jaksel Super Strategis</t>
         </is>
       </c>
       <c r="C1018" t="n">
-        <v>7700000000</v>
+        <v>6900000000</v>
       </c>
       <c r="D1018" t="n">
-        <v>500</v>
+        <v>375</v>
       </c>
       <c r="E1018" t="n">
-        <v>400</v>
+        <v>76</v>
       </c>
       <c r="F1018" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1018" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1018" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1019">
@@ -28957,23 +28957,23 @@
       </c>
       <c r="B1019" t="inlineStr">
         <is>
-          <t>For Sale Rumah Mewah 4 Lantai Kondisi Baru di Pusat Jakarta Selatan Dekat SCBD Senopati</t>
+          <t>Dijual Cepat Rumah Bona Indah Lokasi Strategis Dekat Mrt, Sekolah Sis, Cikal , Al Izhar Rs Mayapadalokasi Stategis Shm</t>
         </is>
       </c>
       <c r="C1019" t="n">
-        <v>6900000000</v>
+        <v>5700000000</v>
       </c>
       <c r="D1019" t="n">
-        <v>375</v>
+        <v>150</v>
       </c>
       <c r="E1019" t="n">
-        <v>76</v>
+        <v>300</v>
       </c>
       <c r="F1019" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1019" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H1019" t="n">
         <v>2</v>
@@ -28985,26 +28985,26 @@
       </c>
       <c r="B1020" t="inlineStr">
         <is>
-          <t>Padmavilla Pejaten</t>
+          <t>Rumah Hitung Tanah di Jagakarsa, Ada Halaman Luas, Mall</t>
         </is>
       </c>
       <c r="C1020" t="n">
-        <v>2600000000</v>
+        <v>19000000000</v>
       </c>
       <c r="D1020" t="n">
-        <v>88</v>
+        <v>300</v>
       </c>
       <c r="E1020" t="n">
-        <v>55</v>
+        <v>2448</v>
       </c>
       <c r="F1020" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1020" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1020" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1021">
@@ -29013,20 +29013,20 @@
       </c>
       <c r="B1021" t="inlineStr">
         <is>
-          <t>Rumah Senopati Kebayoran Baru Rumah di Senopati SHM</t>
+          <t>Rumah di Belakang Aeon Tanjung Barat, Semi Furnished</t>
         </is>
       </c>
       <c r="C1021" t="n">
-        <v>15500000000</v>
+        <v>2750000000</v>
       </c>
       <c r="D1021" t="n">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="E1021" t="n">
-        <v>317</v>
+        <v>150</v>
       </c>
       <c r="F1021" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1021" t="n">
         <v>3</v>
@@ -29041,23 +29041,23 @@
       </c>
       <c r="B1022" t="inlineStr">
         <is>
-          <t>For Sale Rumah Mewah 4 Lantai Kondisi Baru di Jaksel Super Strategis</t>
+          <t>Rumah di Cilandak, 6 KT, Taman, Dekat MRT &amp; Poins</t>
         </is>
       </c>
       <c r="C1022" t="n">
-        <v>6900000000</v>
+        <v>5800000000</v>
       </c>
       <c r="D1022" t="n">
-        <v>375</v>
+        <v>206</v>
       </c>
       <c r="E1022" t="n">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="F1022" t="n">
         <v>4</v>
       </c>
       <c r="G1022" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1022" t="n">
         <v>2</v>
@@ -29069,26 +29069,26 @@
       </c>
       <c r="B1023" t="inlineStr">
         <is>
-          <t>Rumah Mewah Baru 4 Lantai Ada Lift di Pusat Jaksel Lokasi Strategis</t>
+          <t>Rumah asri di Bumi Bintaro Permai 5 KT SHM</t>
         </is>
       </c>
       <c r="C1023" t="n">
-        <v>6900000000</v>
+        <v>6800000000</v>
       </c>
       <c r="D1023" t="n">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="E1023" t="n">
-        <v>76</v>
+        <v>475</v>
       </c>
       <c r="F1023" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1023" t="n">
         <v>4</v>
       </c>
       <c r="H1023" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1024">
@@ -29097,26 +29097,26 @@
       </c>
       <c r="B1024" t="inlineStr">
         <is>
-          <t>Padmavilla Cilandak</t>
+          <t>Rumah di Bukit Duri Dekat LRT, Mall Kokas &amp; Eco Park</t>
         </is>
       </c>
       <c r="C1024" t="n">
-        <v>2830000000</v>
+        <v>3500000000</v>
       </c>
       <c r="D1024" t="n">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="E1024" t="n">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="F1024" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1024" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1024" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1025">
@@ -29125,26 +29125,26 @@
       </c>
       <c r="B1025" t="inlineStr">
         <is>
-          <t>For Sale Rumah Mewah Kondisi Baru di Tengah Jaksel 4 Lantai</t>
+          <t>Rumah Semi Furnished di Pondok Indah, Dekat PIM &amp; MRT</t>
         </is>
       </c>
       <c r="C1025" t="n">
-        <v>6900000000</v>
+        <v>7000000000</v>
       </c>
       <c r="D1025" t="n">
-        <v>375</v>
+        <v>280</v>
       </c>
       <c r="E1025" t="n">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="F1025" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1025" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1025" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1026">
@@ -29153,26 +29153,26 @@
       </c>
       <c r="B1026" t="inlineStr">
         <is>
-          <t>Dijual Cepat Rumah Bona Indah Lokasi Strategis Dekat Mrt, Sekolah Sis, Cikal , Al Izhar Rs Mayapadalokasi Stategis Shm</t>
+          <t>[ Harga Mendekati Njop ] Tebet Barat Commercial Use</t>
         </is>
       </c>
       <c r="C1026" t="n">
-        <v>5700000000</v>
+        <v>13700000000</v>
       </c>
       <c r="D1026" t="n">
-        <v>150</v>
+        <v>520</v>
       </c>
       <c r="E1026" t="n">
-        <v>300</v>
+        <v>528</v>
       </c>
       <c r="F1026" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1026" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H1026" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1027">
@@ -29181,26 +29181,26 @@
       </c>
       <c r="B1027" t="inlineStr">
         <is>
-          <t>Rumah Hitung Tanah di Jagakarsa, Ada Halaman Luas, Mall</t>
+          <t>[ Tebet Barat Akses Lebar ] Bangunan 2025</t>
         </is>
       </c>
       <c r="C1027" t="n">
-        <v>19000000000</v>
+        <v>5750000000</v>
       </c>
       <c r="D1027" t="n">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="E1027" t="n">
-        <v>2448</v>
+        <v>132</v>
       </c>
       <c r="F1027" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G1027" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1027" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1028">
@@ -29209,23 +29209,23 @@
       </c>
       <c r="B1028" t="inlineStr">
         <is>
-          <t>Rumah di Belakang Aeon Tanjung Barat, Semi Furnished</t>
+          <t>[ Rumah Kantor Tebet Barat ] Cocok Untuk Bisnis Maupun Rumah</t>
         </is>
       </c>
       <c r="C1028" t="n">
-        <v>2750000000</v>
+        <v>16500000000</v>
       </c>
       <c r="D1028" t="n">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="E1028" t="n">
-        <v>150</v>
+        <v>502</v>
       </c>
       <c r="F1028" t="n">
         <v>5</v>
       </c>
       <c r="G1028" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1028" t="n">
         <v>1</v>
@@ -29237,26 +29237,26 @@
       </c>
       <c r="B1029" t="inlineStr">
         <is>
-          <t>Rumah Mewah + Rooftop Dekat Toll Di Jl. Moh. Kahfi 1, Jagakarsa Jaksel</t>
+          <t>[ Akses 2 Mobil Tebet Barat ] Best Price Dekat Taman</t>
         </is>
       </c>
       <c r="C1029" t="n">
-        <v>2750000000</v>
+        <v>5000000000</v>
       </c>
       <c r="D1029" t="n">
+        <v>350</v>
+      </c>
+      <c r="E1029" t="n">
         <v>220</v>
       </c>
-      <c r="E1029" t="n">
-        <v>114</v>
-      </c>
       <c r="F1029" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1029" t="n">
         <v>4</v>
       </c>
       <c r="H1029" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1030">
@@ -29265,26 +29265,26 @@
       </c>
       <c r="B1030" t="inlineStr">
         <is>
-          <t>Rumah + Rooftop Siap Huni Deket Toll Brigif Di Jagakarsa Jaksel</t>
+          <t>[ Tebet Barat Commercial Use ] Akses Jalan Utama. Banyak Kafe &amp; Resto Di Area Ini</t>
         </is>
       </c>
       <c r="C1030" t="n">
-        <v>1830000000</v>
+        <v>13500000000</v>
       </c>
       <c r="D1030" t="n">
-        <v>140</v>
+        <v>466</v>
       </c>
       <c r="E1030" t="n">
-        <v>67</v>
+        <v>496</v>
       </c>
       <c r="F1030" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1030" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1030" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1031">
@@ -29293,26 +29293,26 @@
       </c>
       <c r="B1031" t="inlineStr">
         <is>
-          <t>Rumah di Cilandak, 6 KT, Taman, Dekat MRT &amp; Poins</t>
+          <t>( Best Price On The Market ) Cocok Bangun Kost Premium Tebet</t>
         </is>
       </c>
       <c r="C1031" t="n">
-        <v>5800000000</v>
+        <v>7000000000</v>
       </c>
       <c r="D1031" t="n">
-        <v>206</v>
+        <v>432</v>
       </c>
       <c r="E1031" t="n">
-        <v>200</v>
+        <v>432</v>
       </c>
       <c r="F1031" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G1031" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H1031" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1032">
@@ -29321,26 +29321,26 @@
       </c>
       <c r="B1032" t="inlineStr">
         <is>
-          <t>Rumah asri di Bumi Bintaro Permai 5 KT SHM</t>
+          <t>Rumah Tanah Luas Siap Huni Dalam Komplek Asri Di Selatan Jakarta</t>
         </is>
       </c>
       <c r="C1032" t="n">
-        <v>6800000000</v>
+        <v>1390000000</v>
       </c>
       <c r="D1032" t="n">
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="E1032" t="n">
-        <v>475</v>
+        <v>125</v>
       </c>
       <c r="F1032" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1032" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H1032" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1033">
@@ -29349,26 +29349,26 @@
       </c>
       <c r="B1033" t="inlineStr">
         <is>
-          <t>Rumah di Bukit Duri Dekat LRT, Mall Kokas &amp; Eco Park</t>
+          <t>Rumah 3 Lantai Siap Huni Semi Furnished, Jagakarsa</t>
         </is>
       </c>
       <c r="C1033" t="n">
         <v>3500000000</v>
       </c>
       <c r="D1033" t="n">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="E1033" t="n">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F1033" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1033" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1033" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1034">
@@ -29377,26 +29377,26 @@
       </c>
       <c r="B1034" t="inlineStr">
         <is>
-          <t>Rumah Murah Classic Modern Tebet Mas Spesifikasi Mahal Siap Huni Jual Cepat Lihat Jamin Beli</t>
+          <t>Rumah Elegan, Harga Menggoda, Kesempatan Tak Terulang !</t>
         </is>
       </c>
       <c r="C1034" t="n">
-        <v>15500000000</v>
+        <v>1170000000</v>
       </c>
       <c r="D1034" t="n">
-        <v>340</v>
+        <v>56</v>
       </c>
       <c r="E1034" t="n">
-        <v>350</v>
+        <v>29</v>
       </c>
       <c r="F1034" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1034" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H1034" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1035">
@@ -29405,26 +29405,26 @@
       </c>
       <c r="B1035" t="inlineStr">
         <is>
-          <t>Rumah Semi Furnished di Pondok Indah, Dekat PIM &amp; MRT</t>
+          <t>Murah Jual Nego Cepat Rumah Mewah+ Pool 634m2 Di Pondok Indah</t>
         </is>
       </c>
       <c r="C1035" t="n">
-        <v>7000000000</v>
+        <v>44000000000</v>
       </c>
       <c r="D1035" t="n">
-        <v>280</v>
+        <v>720</v>
       </c>
       <c r="E1035" t="n">
-        <v>120</v>
+        <v>634</v>
       </c>
       <c r="F1035" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1035" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1035" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1036">
@@ -29433,26 +29433,26 @@
       </c>
       <c r="B1036" t="inlineStr">
         <is>
-          <t>[ Harga Mendekati Njop ] Tebet Barat Commercial Use</t>
+          <t>Rumah di Darmawangsa, Kebayoran Baru, Akses jalan 3 mobil, 1 km ke MRT Blok A</t>
         </is>
       </c>
       <c r="C1036" t="n">
-        <v>13700000000</v>
+        <v>22000000000</v>
       </c>
       <c r="D1036" t="n">
-        <v>520</v>
+        <v>360</v>
       </c>
       <c r="E1036" t="n">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="F1036" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1036" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1036" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1037">
@@ -29461,26 +29461,26 @@
       </c>
       <c r="B1037" t="inlineStr">
         <is>
-          <t>[ Tebet Barat Akses Lebar ] Bangunan 2025</t>
+          <t>Rumah Super Mewah Furnished di Area Premium di Kebayoran Baru, Turun Harga</t>
         </is>
       </c>
       <c r="C1037" t="n">
-        <v>5750000000</v>
+        <v>79900000000</v>
       </c>
       <c r="D1037" t="n">
-        <v>270</v>
+        <v>750</v>
       </c>
       <c r="E1037" t="n">
-        <v>132</v>
+        <v>1026</v>
       </c>
       <c r="F1037" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G1037" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1037" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1038">
@@ -29489,26 +29489,26 @@
       </c>
       <c r="B1038" t="inlineStr">
         <is>
-          <t>[ Rumah Kantor Tebet Barat ] Cocok Untuk Bisnis Maupun Rumah</t>
+          <t>Rumah Baru Siaphuni Deket Mrt Lebak Bulus Dalam Cluster Dekat Tol</t>
         </is>
       </c>
       <c r="C1038" t="n">
-        <v>16500000000</v>
+        <v>2000000000</v>
       </c>
       <c r="D1038" t="n">
-        <v>350</v>
+        <v>134</v>
       </c>
       <c r="E1038" t="n">
-        <v>502</v>
+        <v>127</v>
       </c>
       <c r="F1038" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1038" t="n">
         <v>4</v>
       </c>
       <c r="H1038" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1039">
@@ -29517,26 +29517,26 @@
       </c>
       <c r="B1039" t="inlineStr">
         <is>
-          <t>[ Akses 2 Mobil Tebet Barat ] Best Price Dekat Taman</t>
+          <t>Rumah 4 Lantai Private Poll Di Jagakarsa Jakarta Selatan Cluster</t>
         </is>
       </c>
       <c r="C1039" t="n">
-        <v>5000000000</v>
+        <v>3850000000</v>
       </c>
       <c r="D1039" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="E1039" t="n">
-        <v>220</v>
+        <v>102</v>
       </c>
       <c r="F1039" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1039" t="n">
         <v>4</v>
       </c>
       <c r="H1039" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1040">
@@ -29545,17 +29545,17 @@
       </c>
       <c r="B1040" t="inlineStr">
         <is>
-          <t>[ Tebet Barat Commercial Use ] Akses Jalan Utama. Banyak Kafe &amp; Resto Di Area Ini</t>
+          <t>Rumah Siaphuni Di Pondok Indah 3 Lantai Dekat Mall Tol Rumahsakit</t>
         </is>
       </c>
       <c r="C1040" t="n">
-        <v>13500000000</v>
+        <v>8000000000</v>
       </c>
       <c r="D1040" t="n">
-        <v>466</v>
+        <v>430</v>
       </c>
       <c r="E1040" t="n">
-        <v>496</v>
+        <v>250</v>
       </c>
       <c r="F1040" t="n">
         <v>5</v>
@@ -29564,7 +29564,7 @@
         <v>5</v>
       </c>
       <c r="H1040" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1041">
@@ -29573,26 +29573,26 @@
       </c>
       <c r="B1041" t="inlineStr">
         <is>
-          <t>( Best Price On The Market ) Cocok Bangun Kost Premium Tebet</t>
+          <t>Rumah Mewah Di Pondok Indah Area Id 9843</t>
         </is>
       </c>
       <c r="C1041" t="n">
-        <v>7000000000</v>
+        <v>45000000000</v>
       </c>
       <c r="D1041" t="n">
-        <v>432</v>
+        <v>1800</v>
       </c>
       <c r="E1041" t="n">
-        <v>432</v>
+        <v>1225</v>
       </c>
       <c r="F1041" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1041" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1041" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1042">
@@ -29601,23 +29601,23 @@
       </c>
       <c r="B1042" t="inlineStr">
         <is>
-          <t>Rumah Tanah Luas Siap Huni Dalam Komplek Asri Di Selatan Jakarta</t>
+          <t>Rumah Strategis Di Tengah Kota</t>
         </is>
       </c>
       <c r="C1042" t="n">
-        <v>1390000000</v>
+        <v>7800000000</v>
       </c>
       <c r="D1042" t="n">
-        <v>90</v>
+        <v>350</v>
       </c>
       <c r="E1042" t="n">
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="F1042" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1042" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1042" t="n">
         <v>2</v>
@@ -29629,26 +29629,26 @@
       </c>
       <c r="B1043" t="inlineStr">
         <is>
-          <t>Rumah 3 Lantai Siap Huni Semi Furnished, Jagakarsa</t>
+          <t>Nivara Resort Townhouse at Wijaya</t>
         </is>
       </c>
       <c r="C1043" t="n">
-        <v>3500000000</v>
+        <v>7090000000</v>
       </c>
       <c r="D1043" t="n">
-        <v>230</v>
+        <v>375</v>
       </c>
       <c r="E1043" t="n">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="F1043" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1043" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H1043" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1044">
@@ -29657,26 +29657,26 @@
       </c>
       <c r="B1044" t="inlineStr">
         <is>
-          <t>Rumah Elegan, Harga Menggoda, Kesempatan Tak Terulang !</t>
+          <t>Harga Paling Kompetitif Di Kemang, Jakarta Selatan</t>
         </is>
       </c>
       <c r="C1044" t="n">
-        <v>1170000000</v>
+        <v>9000000000</v>
       </c>
       <c r="D1044" t="n">
-        <v>56</v>
+        <v>500</v>
       </c>
       <c r="E1044" t="n">
-        <v>29</v>
+        <v>420</v>
       </c>
       <c r="F1044" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1044" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1044" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1045">
@@ -29685,26 +29685,26 @@
       </c>
       <c r="B1045" t="inlineStr">
         <is>
-          <t>Murah Jual Nego Cepat Rumah Mewah+ Pool 634m2 Di Pondok Indah</t>
+          <t>Rumah 2 Lantai Hook Di Pinang Perak Pondok Indah Shm Lokasi Bagus</t>
         </is>
       </c>
       <c r="C1045" t="n">
-        <v>44000000000</v>
+        <v>16000000000</v>
       </c>
       <c r="D1045" t="n">
-        <v>720</v>
+        <v>616</v>
       </c>
       <c r="E1045" t="n">
-        <v>634</v>
+        <v>383</v>
       </c>
       <c r="F1045" t="n">
         <v>4</v>
       </c>
       <c r="G1045" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H1045" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1046">
@@ -29713,23 +29713,23 @@
       </c>
       <c r="B1046" t="inlineStr">
         <is>
-          <t>Rumah di Darmawangsa, Kebayoran Baru, Akses jalan 3 mobil, 1 km ke MRT Blok A</t>
+          <t>Rumah 2 Lantai Di Cilandak Fatmawati Dekat Ke Stasiun Mrt Haji Nawi</t>
         </is>
       </c>
       <c r="C1046" t="n">
-        <v>22000000000</v>
+        <v>7700000000</v>
       </c>
       <c r="D1046" t="n">
-        <v>360</v>
+        <v>216</v>
       </c>
       <c r="E1046" t="n">
-        <v>518</v>
+        <v>270</v>
       </c>
       <c r="F1046" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1046" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1046" t="n">
         <v>2</v>
@@ -29741,26 +29741,26 @@
       </c>
       <c r="B1047" t="inlineStr">
         <is>
-          <t>Rumah Super Mewah Furnished di Area Premium di Kebayoran Baru, Turun Harga</t>
+          <t>Rumah Mewah Baru 4 Lantai Ada Lift di Pusat Jaksel Lokasi Strategis</t>
         </is>
       </c>
       <c r="C1047" t="n">
-        <v>79900000000</v>
+        <v>6900000000</v>
       </c>
       <c r="D1047" t="n">
-        <v>750</v>
+        <v>375</v>
       </c>
       <c r="E1047" t="n">
-        <v>1026</v>
+        <v>76</v>
       </c>
       <c r="F1047" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G1047" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H1047" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1048">
@@ -29769,26 +29769,26 @@
       </c>
       <c r="B1048" t="inlineStr">
         <is>
-          <t>Dijual Rumah Exclusive Di Kawasan Elit Kemang Jaksel</t>
+          <t>For Sale Rumah Mewah Kondisi Baru di Tengah Jaksel 4 Lantai</t>
         </is>
       </c>
       <c r="C1048" t="n">
-        <v>13500000000</v>
+        <v>6900000000</v>
       </c>
       <c r="D1048" t="n">
-        <v>325</v>
+        <v>375</v>
       </c>
       <c r="E1048" t="n">
-        <v>696</v>
+        <v>76</v>
       </c>
       <c r="F1048" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1048" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1048" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1049">
@@ -29797,23 +29797,23 @@
       </c>
       <c r="B1049" t="inlineStr">
         <is>
-          <t>Rumah Baru Siaphuni Deket Mrt Lebak Bulus Dalam Cluster Dekat Tol</t>
+          <t>ZENITPARC HYATT</t>
         </is>
       </c>
       <c r="C1049" t="n">
-        <v>2000000000</v>
+        <v>2400000000</v>
       </c>
       <c r="D1049" t="n">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E1049" t="n">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F1049" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1049" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1049" t="n">
         <v>2</v>
@@ -29825,26 +29825,26 @@
       </c>
       <c r="B1050" t="inlineStr">
         <is>
-          <t>Rumah 4 Lantai Private Poll Di Jagakarsa Jakarta Selatan Cluster</t>
+          <t>- Murah !! Dijual Cepat !! Rumah Siap Huni 10x25 dibawah NJOP di Niaga Hijau Pondok Indah</t>
         </is>
       </c>
       <c r="C1050" t="n">
-        <v>3850000000</v>
+        <v>5700000000</v>
       </c>
       <c r="D1050" t="n">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="E1050" t="n">
-        <v>102</v>
+        <v>250</v>
       </c>
       <c r="F1050" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1050" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1050" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1051">
@@ -29853,23 +29853,23 @@
       </c>
       <c r="B1051" t="inlineStr">
         <is>
-          <t>Rumah Siaphuni Di Pondok Indah 3 Lantai Dekat Mall Tol Rumahsakit</t>
+          <t>Rumah Murah Classic Modern Tebet Mas Spesifikasi Mahal Siap Huni Jual Cepat Lihat Jamin Beli</t>
         </is>
       </c>
       <c r="C1051" t="n">
-        <v>8000000000</v>
+        <v>15500000000</v>
       </c>
       <c r="D1051" t="n">
-        <v>430</v>
+        <v>340</v>
       </c>
       <c r="E1051" t="n">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="F1051" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1051" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1051" t="n">
         <v>3</v>
@@ -29881,26 +29881,950 @@
       </c>
       <c r="B1052" t="inlineStr">
         <is>
-          <t>Rumah Mewah Di Pondok Indah Area Id 9843</t>
+          <t>For Sale Rumah Hitung Tanah Tebet</t>
         </is>
       </c>
       <c r="C1052" t="n">
-        <v>45000000000</v>
+        <v>1500000000</v>
       </c>
       <c r="D1052" t="n">
-        <v>1800</v>
+        <v>75</v>
       </c>
       <c r="E1052" t="n">
-        <v>1225</v>
+        <v>81</v>
       </c>
       <c r="F1052" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1052" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H1052" t="n">
-        <v>4</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="n">
+        <v>1052</v>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Padmavilla Pejaten</t>
+        </is>
+      </c>
+      <c r="C1053" t="n">
+        <v>2600000000</v>
+      </c>
+      <c r="D1053" t="n">
+        <v>88</v>
+      </c>
+      <c r="E1053" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1053" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1053" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1053" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="n">
+        <v>1053</v>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>RUMAH TEBET TURUN HARGA JADI  8.1 M DEKAT NJOP</t>
+        </is>
+      </c>
+      <c r="C1054" t="n">
+        <v>7700000000</v>
+      </c>
+      <c r="D1054" t="n">
+        <v>500</v>
+      </c>
+      <c r="E1054" t="n">
+        <v>400</v>
+      </c>
+      <c r="F1054" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1054" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1054" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="n">
+        <v>1054</v>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>RUMAH KOST 10 PINTU DI TEBET ! GOOD INVEST</t>
+        </is>
+      </c>
+      <c r="C1055" t="n">
+        <v>2500000000</v>
+      </c>
+      <c r="D1055" t="n">
+        <v>250</v>
+      </c>
+      <c r="E1055" t="n">
+        <v>130</v>
+      </c>
+      <c r="F1055" t="n">
+        <v>10</v>
+      </c>
+      <c r="G1055" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1055" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="n">
+        <v>1055</v>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>SHM 198 M2 ! 16 JT PERMETER AKSES 2 MOBIL DI TEBET, DEKAT MALL KOKAS</t>
+        </is>
+      </c>
+      <c r="C1056" t="n">
+        <v>3200000000</v>
+      </c>
+      <c r="D1056" t="n">
+        <v>250</v>
+      </c>
+      <c r="E1056" t="n">
+        <v>198</v>
+      </c>
+      <c r="F1056" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1056" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1056" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="n">
+        <v>1056</v>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Padmavilla Cilandak</t>
+        </is>
+      </c>
+      <c r="C1057" t="n">
+        <v>2830000000</v>
+      </c>
+      <c r="D1057" t="n">
+        <v>112</v>
+      </c>
+      <c r="E1057" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1057" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1057" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1057" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="n">
+        <v>1057</v>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>AKSES 3 MOBIL - RUMAH MEWAH DI TEBET TIMUR ( SEMI FURNISHED )</t>
+        </is>
+      </c>
+      <c r="C1058" t="n">
+        <v>13000000000</v>
+      </c>
+      <c r="D1058" t="n">
+        <v>250</v>
+      </c>
+      <c r="E1058" t="n">
+        <v>318</v>
+      </c>
+      <c r="F1058" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1058" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1058" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="n">
+        <v>1058</v>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>1 M An ! ( Dekat Akses 3 Mobil) Tebet Barat</t>
+        </is>
+      </c>
+      <c r="C1059" t="n">
+        <v>1550000000</v>
+      </c>
+      <c r="D1059" t="n">
+        <v>100</v>
+      </c>
+      <c r="E1059" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1059" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1059" t="n">
+        <v>2</v>
+      </c>
+      <c r="H1059" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="n">
+        <v>1059</v>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Dibawah Njop Kemang Rumah Klassik Tidak Banjir</t>
+        </is>
+      </c>
+      <c r="C1060" t="n">
+        <v>27000000000</v>
+      </c>
+      <c r="D1060" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E1060" t="n">
+        <v>2028</v>
+      </c>
+      <c r="F1060" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1060" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1060" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="n">
+        <v>1060</v>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>BEST PRICE TEBET ! AKSES LEBAR, RUMAH SIAP HUNI</t>
+        </is>
+      </c>
+      <c r="C1061" t="n">
+        <v>7700000000</v>
+      </c>
+      <c r="D1061" t="n">
+        <v>600</v>
+      </c>
+      <c r="E1061" t="n">
+        <v>400</v>
+      </c>
+      <c r="F1061" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1061" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1061" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="n">
+        <v>1061</v>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Dijual Cepat Rumah Tebet Jak-sel</t>
+        </is>
+      </c>
+      <c r="C1062" t="n">
+        <v>24000000000</v>
+      </c>
+      <c r="D1062" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E1062" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F1062" t="n">
+        <v>8</v>
+      </c>
+      <c r="G1062" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1062" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="n">
+        <v>1062</v>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Harus Terjual!! Murah Kios Ruko Dikalibata Strategis</t>
+        </is>
+      </c>
+      <c r="C1063" t="n">
+        <v>3000000000</v>
+      </c>
+      <c r="D1063" t="n">
+        <v>180</v>
+      </c>
+      <c r="E1063" t="n">
+        <v>230</v>
+      </c>
+      <c r="F1063" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1063" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1063" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="n">
+        <v>1063</v>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Rumah Siap Huni Murah Hanya 7 Menit Jalan Kaki Dari Mrt Fatmawati</t>
+        </is>
+      </c>
+      <c r="C1064" t="n">
+        <v>2600000000</v>
+      </c>
+      <c r="D1064" t="n">
+        <v>135</v>
+      </c>
+      <c r="E1064" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1064" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1064" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1064" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="n">
+        <v>1064</v>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Dijual Cepat Rumah Pondok Indah Luxurious Modern Classic, Premium Area, Siap Huni</t>
+        </is>
+      </c>
+      <c r="C1065" t="n">
+        <v>21000000000</v>
+      </c>
+      <c r="D1065" t="n">
+        <v>700</v>
+      </c>
+      <c r="E1065" t="n">
+        <v>353</v>
+      </c>
+      <c r="F1065" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1065" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1065" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="n">
+        <v>1065</v>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Dijual Rumah Mewah di Pondok Indah .</t>
+        </is>
+      </c>
+      <c r="C1066" t="n">
+        <v>33000000000</v>
+      </c>
+      <c r="D1066" t="n">
+        <v>750</v>
+      </c>
+      <c r="E1066" t="n">
+        <v>607</v>
+      </c>
+      <c r="F1066" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1066" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1066" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="n">
+        <v>1066</v>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>For Sale Rumah Mewah 4 Lantai Kondisi Baru di Tengah Jaksel Dekat SCBD</t>
+        </is>
+      </c>
+      <c r="C1067" t="n">
+        <v>6900000000</v>
+      </c>
+      <c r="D1067" t="n">
+        <v>375</v>
+      </c>
+      <c r="E1067" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1067" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1067" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1067" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="n">
+        <v>1067</v>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Dijual Rumah Siap Huni Lokasi Sangat Strategis Di Jl. Ciniru, Kebayoran Baru, Jak-sel Rumah Bagus SHM</t>
+        </is>
+      </c>
+      <c r="C1068" t="n">
+        <v>18500000000</v>
+      </c>
+      <c r="D1068" t="n">
+        <v>245</v>
+      </c>
+      <c r="E1068" t="n">
+        <v>260</v>
+      </c>
+      <c r="F1068" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1068" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1068" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="n">
+        <v>1068</v>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Jual Rumah Mewah Di Kemang, Jak-sel Dilingkungan Yang Aman Dan Nyaman</t>
+        </is>
+      </c>
+      <c r="C1069" t="n">
+        <v>24500000000</v>
+      </c>
+      <c r="D1069" t="n">
+        <v>600</v>
+      </c>
+      <c r="E1069" t="n">
+        <v>787</v>
+      </c>
+      <c r="F1069" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1069" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1069" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="n">
+        <v>1069</v>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>For Sale Rumah Mewah Kondisi Baru di Tengah Jaksel Dekat SCBD 4 Lantai Jarang Ada</t>
+        </is>
+      </c>
+      <c r="C1070" t="n">
+        <v>6900000000</v>
+      </c>
+      <c r="D1070" t="n">
+        <v>375</v>
+      </c>
+      <c r="E1070" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1070" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1070" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1070" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="n">
+        <v>1070</v>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>For Sale Rumah Mewah Kondisi Baru di Tengah Jaksel Dekat SCBD Jarang Ada</t>
+        </is>
+      </c>
+      <c r="C1071" t="n">
+        <v>6900000000</v>
+      </c>
+      <c r="D1071" t="n">
+        <v>375</v>
+      </c>
+      <c r="E1071" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1071" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1071" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1071" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="n">
+        <v>1071</v>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Rumah Tinggal Jalan Kedondong</t>
+        </is>
+      </c>
+      <c r="C1072" t="n">
+        <v>1470000000</v>
+      </c>
+      <c r="D1072" t="n">
+        <v>300</v>
+      </c>
+      <c r="E1072" t="n">
+        <v>200</v>
+      </c>
+      <c r="F1072" t="n">
+        <v>1</v>
+      </c>
+      <c r="G1072" t="n">
+        <v>1</v>
+      </c>
+      <c r="H1072" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="n">
+        <v>1072</v>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Dijual Rumah Daklam Townhouse Harga Murah Di Cilandak Tb Simatupang Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="C1073" t="n">
+        <v>3500000000</v>
+      </c>
+      <c r="D1073" t="n">
+        <v>250</v>
+      </c>
+      <c r="E1073" t="n">
+        <v>144</v>
+      </c>
+      <c r="F1073" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1073" t="n">
+        <v>2</v>
+      </c>
+      <c r="H1073" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="n">
+        <v>1073</v>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Rumah Mewah Kondisi Baru di Jakarta Selatan 4 Lantai</t>
+        </is>
+      </c>
+      <c r="C1074" t="n">
+        <v>6900000000</v>
+      </c>
+      <c r="D1074" t="n">
+        <v>375</v>
+      </c>
+      <c r="E1074" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1074" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1074" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1074" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="n">
+        <v>1074</v>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Dijual Rumah Di Tebet Barat Dalam Akses 2 Mobil Tebet Barat Jaksel</t>
+        </is>
+      </c>
+      <c r="C1075" t="n">
+        <v>7700000000</v>
+      </c>
+      <c r="D1075" t="n">
+        <v>500</v>
+      </c>
+      <c r="E1075" t="n">
+        <v>400</v>
+      </c>
+      <c r="F1075" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1075" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1075" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="n">
+        <v>1075</v>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Dijual Rumah Exclusive Di Kawasan Elit Kemang Jaksel</t>
+        </is>
+      </c>
+      <c r="C1076" t="n">
+        <v>13500000000</v>
+      </c>
+      <c r="D1076" t="n">
+        <v>325</v>
+      </c>
+      <c r="E1076" t="n">
+        <v>696</v>
+      </c>
+      <c r="F1076" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1076" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1076" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="n">
+        <v>1076</v>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Hunian Cantik Siap Huni Bergaya Scandinavian Modern Akses Jalan Raya Jagakarsa Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="C1077" t="n">
+        <v>2900000000</v>
+      </c>
+      <c r="D1077" t="n">
+        <v>100</v>
+      </c>
+      <c r="E1077" t="n">
+        <v>155</v>
+      </c>
+      <c r="F1077" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1077" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1077" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="n">
+        <v>1077</v>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Rumah Baru Di Pejaten Timur. Pasar Minggu Kota Jakarta Selatan Bebas Banjir, Strategis, Dekat Akses ********</t>
+        </is>
+      </c>
+      <c r="C1078" t="n">
+        <v>1200000000</v>
+      </c>
+      <c r="D1078" t="n">
+        <v>81</v>
+      </c>
+      <c r="E1078" t="n">
+        <v>54</v>
+      </c>
+      <c r="F1078" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1078" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1078" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="n">
+        <v>1078</v>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>View Golf Private Swimming Pool Pondok Indah Siap Huni Asri Tenang Bebas Banjir Kirim Loi</t>
+        </is>
+      </c>
+      <c r="C1079" t="n">
+        <v>170000000000</v>
+      </c>
+      <c r="D1079" t="n">
+        <v>1400</v>
+      </c>
+      <c r="E1079" t="n">
+        <v>2835</v>
+      </c>
+      <c r="F1079" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1079" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1079" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="n">
+        <v>1079</v>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Brand New Modern American Classic House Pondok Indah</t>
+        </is>
+      </c>
+      <c r="C1080" t="n">
+        <v>35000000000</v>
+      </c>
+      <c r="D1080" t="n">
+        <v>750</v>
+      </c>
+      <c r="E1080" t="n">
+        <v>406</v>
+      </c>
+      <c r="F1080" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1080" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1080" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="n">
+        <v>1080</v>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Turun Harga ! Rumah Nyaman &amp; Aman 2 Lantai Depan Taman</t>
+        </is>
+      </c>
+      <c r="C1081" t="n">
+        <v>3000000000</v>
+      </c>
+      <c r="D1081" t="n">
+        <v>190</v>
+      </c>
+      <c r="E1081" t="n">
+        <v>135</v>
+      </c>
+      <c r="F1081" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1081" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1081" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="n">
+        <v>1081</v>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Rumah Murah di Gandaria Kebayoran Baru, SHM, 6Kt</t>
+        </is>
+      </c>
+      <c r="C1082" t="n">
+        <v>11500000000</v>
+      </c>
+      <c r="D1082" t="n">
+        <v>400</v>
+      </c>
+      <c r="E1082" t="n">
+        <v>580</v>
+      </c>
+      <c r="F1082" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1082" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1082" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="n">
+        <v>1082</v>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Rumah Mewah + Rooftop Dekat Toll Di Jl. Moh. Kahfi 1, Jagakarsa Jaksel</t>
+        </is>
+      </c>
+      <c r="C1083" t="n">
+        <v>2750000000</v>
+      </c>
+      <c r="D1083" t="n">
+        <v>220</v>
+      </c>
+      <c r="E1083" t="n">
+        <v>114</v>
+      </c>
+      <c r="F1083" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1083" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1083" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="n">
+        <v>1083</v>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Rumah + Rooftop Siap Huni Deket Toll Brigif Di Jagakarsa Jaksel</t>
+        </is>
+      </c>
+      <c r="C1084" t="n">
+        <v>1830000000</v>
+      </c>
+      <c r="D1084" t="n">
+        <v>140</v>
+      </c>
+      <c r="E1084" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1084" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1084" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1084" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="n">
+        <v>1084</v>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>For Sale Rumah Mewah 4 LT Kondisi Baru di Pusat Jakarta Selatan Lokasi Strategis</t>
+        </is>
+      </c>
+      <c r="C1085" t="n">
+        <v>6900000000</v>
+      </c>
+      <c r="D1085" t="n">
+        <v>375</v>
+      </c>
+      <c r="E1085" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1085" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1085" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1085" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>